<commit_message>
Fix bug in auto_run.sh
</commit_message>
<xml_diff>
--- a/conf/excel/C_N.xlsx
+++ b/conf/excel/C_N.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\配置文件相关\newCA-config-clear\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A2F499-6CDA-4211-B210-EF050897DBBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12390"/>
+    <workbookView xWindow="5220" yWindow="2280" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_N_New.conf" sheetId="2" r:id="rId1"/>
@@ -146,18 +147,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>catalog=010A10;&lt;SetCoord&gt;(C_N, , subnodeid, id)-&gt;GEOMETRY</t>
+    <t>生成C_TrafficLight并进行路口居中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生成C_TrafficLight并进行路口居中</t>
+    <t>catalog=010A10;&lt;SetCoord&gt;(C_N, , subnodeid, id)-&gt;GEOMETRY@FullAvg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,10 +251,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -535,11 +536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -550,18 +551,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -578,11 +579,11 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -597,7 +598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -612,18 +613,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>